<commit_message>
Commiting the changes in Riddles automation for date logic
</commit_message>
<xml_diff>
--- a/Application Open/Riddles_with_Answer.xlsx
+++ b/Application Open/Riddles_with_Answer.xlsx
@@ -12,14 +12,14 @@
     <x:sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="122211"/>
+  <x:calcPr calcId="124519"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="326">
   <x:si>
-    <x:t>Riddles</x:t>
+    <x:t>Riddles with answers</x:t>
   </x:si>
   <x:si>
     <x:t>ஓடுவான், வருவான்; ஒற்றைக் காலில் நிற்பான். அவன் யார்? Ans:-கதவு</x:t>
@@ -1045,8 +1045,9 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -1347,1674 +1348,1674 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:A333"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="1" spans="1:1">
-      <x:c r="A1" s="1" t="s">
+      <x:c r="A1" s="2" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:1">
-      <x:c r="A2" s="1" t="s">
+      <x:c r="A2" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:1">
-      <x:c r="A3" s="1" t="s">
+      <x:c r="A3" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:1">
-      <x:c r="A4" s="1" t="s">
+      <x:c r="A4" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:1">
-      <x:c r="A5" s="1" t="s">
+      <x:c r="A5" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:1">
-      <x:c r="A6" s="1" t="s">
+      <x:c r="A6" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:1">
-      <x:c r="A7" s="1" t="s">
+      <x:c r="A7" s="2" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:1">
-      <x:c r="A8" s="1" t="s">
+      <x:c r="A8" s="2" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:1">
-      <x:c r="A9" s="1" t="s">
+      <x:c r="A9" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:1">
-      <x:c r="A10" s="1" t="s">
+      <x:c r="A10" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:1">
-      <x:c r="A11" s="1" t="s">
+      <x:c r="A11" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:1">
-      <x:c r="A12" s="1" t="s">
+      <x:c r="A12" s="2" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:1">
-      <x:c r="A13" s="1" t="s">
+      <x:c r="A13" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:1">
-      <x:c r="A14" s="1" t="s">
+      <x:c r="A14" s="2" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:1">
-      <x:c r="A15" s="1" t="s">
+      <x:c r="A15" s="2" t="s">
         <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:1">
-      <x:c r="A16" s="1" t="s">
+      <x:c r="A16" s="2" t="s">
         <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:1">
-      <x:c r="A17" s="1" t="s">
+      <x:c r="A17" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:1">
-      <x:c r="A18" s="1" t="s">
+      <x:c r="A18" s="2" t="s">
         <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:1">
-      <x:c r="A19" s="1" t="s">
+      <x:c r="A19" s="2" t="s">
         <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:1">
-      <x:c r="A20" s="1" t="s">
+      <x:c r="A20" s="2" t="s">
         <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:1">
-      <x:c r="A21" s="1" t="s">
+      <x:c r="A21" s="2" t="s">
         <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:1">
-      <x:c r="A22" s="1" t="s">
+      <x:c r="A22" s="2" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:1">
-      <x:c r="A23" s="1" t="s">
+      <x:c r="A23" s="2" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:1">
-      <x:c r="A24" s="1" t="s">
+      <x:c r="A24" s="2" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:1">
-      <x:c r="A25" s="1" t="s">
+      <x:c r="A25" s="2" t="s">
         <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:1">
-      <x:c r="A26" s="1" t="s">
+      <x:c r="A26" s="2" t="s">
         <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:1">
-      <x:c r="A27" s="1" t="s">
+      <x:c r="A27" s="2" t="s">
         <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:1">
-      <x:c r="A28" s="1" t="s">
+      <x:c r="A28" s="2" t="s">
         <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:1">
-      <x:c r="A29" s="1" t="s">
+      <x:c r="A29" s="2" t="s">
         <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:1">
-      <x:c r="A30" s="1" t="s">
+      <x:c r="A30" s="2" t="s">
         <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:1">
-      <x:c r="A31" s="1" t="s">
+      <x:c r="A31" s="2" t="s">
         <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:1">
-      <x:c r="A32" s="1" t="s">
+      <x:c r="A32" s="2" t="s">
         <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:1">
-      <x:c r="A33" s="1" t="s">
+      <x:c r="A33" s="2" t="s">
         <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:1">
-      <x:c r="A34" s="1" t="s">
+      <x:c r="A34" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:1">
-      <x:c r="A35" s="1" t="s">
+      <x:c r="A35" s="2" t="s">
         <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:1">
-      <x:c r="A36" s="1" t="s">
+      <x:c r="A36" s="2" t="s">
         <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:1">
-      <x:c r="A37" s="1" t="s">
+      <x:c r="A37" s="2" t="s">
         <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:1">
-      <x:c r="A38" s="1" t="s">
+      <x:c r="A38" s="2" t="s">
         <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:1">
-      <x:c r="A39" s="1" t="s">
+      <x:c r="A39" s="2" t="s">
         <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:1">
-      <x:c r="A40" s="1" t="s">
+      <x:c r="A40" s="2" t="s">
         <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:1">
-      <x:c r="A41" s="1" t="s">
+      <x:c r="A41" s="2" t="s">
         <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:1">
-      <x:c r="A42" s="1" t="s">
+      <x:c r="A42" s="2" t="s">
         <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:1">
-      <x:c r="A43" s="1" t="s">
+      <x:c r="A43" s="2" t="s">
         <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:1">
-      <x:c r="A44" s="1" t="s">
+      <x:c r="A44" s="2" t="s">
         <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:1">
-      <x:c r="A45" s="1" t="s">
+      <x:c r="A45" s="2" t="s">
         <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:1">
-      <x:c r="A46" s="1" t="s">
+      <x:c r="A46" s="2" t="s">
         <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:1">
-      <x:c r="A47" s="1" t="s">
+      <x:c r="A47" s="2" t="s">
         <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:1">
-      <x:c r="A48" s="1" t="s">
+      <x:c r="A48" s="2" t="s">
         <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:1">
-      <x:c r="A49" s="1" t="s">
+      <x:c r="A49" s="2" t="s">
         <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:1">
-      <x:c r="A50" s="1" t="s">
+      <x:c r="A50" s="2" t="s">
         <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:1">
-      <x:c r="A51" s="1" t="s">
+      <x:c r="A51" s="2" t="s">
         <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:1">
-      <x:c r="A52" s="1" t="s">
+      <x:c r="A52" s="2" t="s">
         <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:1">
-      <x:c r="A53" s="1" t="s">
+      <x:c r="A53" s="2" t="s">
         <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:1">
-      <x:c r="A54" s="1" t="s">
+      <x:c r="A54" s="2" t="s">
         <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:1">
-      <x:c r="A55" s="1" t="s">
+      <x:c r="A55" s="2" t="s">
         <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:1">
-      <x:c r="A56" s="1" t="s">
+      <x:c r="A56" s="2" t="s">
         <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:1">
-      <x:c r="A57" s="1" t="s">
+      <x:c r="A57" s="2" t="s">
         <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:1">
-      <x:c r="A58" s="1" t="s">
+      <x:c r="A58" s="2" t="s">
         <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:1">
-      <x:c r="A59" s="1" t="s">
+      <x:c r="A59" s="2" t="s">
         <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:1">
-      <x:c r="A60" s="1" t="s">
+      <x:c r="A60" s="2" t="s">
         <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:1">
-      <x:c r="A61" s="1" t="s">
+      <x:c r="A61" s="2" t="s">
         <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:1">
-      <x:c r="A62" s="1" t="s">
+      <x:c r="A62" s="2" t="s">
         <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:1">
-      <x:c r="A63" s="1" t="s">
+      <x:c r="A63" s="2" t="s">
         <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:1">
-      <x:c r="A64" s="1" t="s">
+      <x:c r="A64" s="2" t="s">
         <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:1">
-      <x:c r="A65" s="1" t="s">
+      <x:c r="A65" s="2" t="s">
         <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:1">
-      <x:c r="A66" s="1" t="s">
+      <x:c r="A66" s="2" t="s">
         <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:1">
-      <x:c r="A67" s="1" t="s">
+      <x:c r="A67" s="2" t="s">
         <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="68" spans="1:1">
-      <x:c r="A68" s="1" t="s">
+      <x:c r="A68" s="2" t="s">
         <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:1">
-      <x:c r="A69" s="1" t="s">
+      <x:c r="A69" s="2" t="s">
         <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="70" spans="1:1">
-      <x:c r="A70" s="1" t="s">
+      <x:c r="A70" s="2" t="s">
         <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="71" spans="1:1">
-      <x:c r="A71" s="1" t="s">
+      <x:c r="A71" s="2" t="s">
         <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:1">
-      <x:c r="A72" s="1" t="s">
+      <x:c r="A72" s="2" t="s">
         <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:1">
-      <x:c r="A73" s="1" t="s">
+      <x:c r="A73" s="2" t="s">
         <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:1">
-      <x:c r="A74" s="1" t="s">
+      <x:c r="A74" s="2" t="s">
         <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:1">
-      <x:c r="A75" s="1" t="s">
+      <x:c r="A75" s="2" t="s">
         <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:1">
-      <x:c r="A76" s="1" t="s">
+      <x:c r="A76" s="2" t="s">
         <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:1">
-      <x:c r="A77" s="1" t="s">
+      <x:c r="A77" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:1">
-      <x:c r="A78" s="1" t="s">
+      <x:c r="A78" s="2" t="s">
         <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:1">
-      <x:c r="A79" s="1" t="s">
+      <x:c r="A79" s="2" t="s">
         <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:1">
-      <x:c r="A80" s="1" t="s">
+      <x:c r="A80" s="2" t="s">
         <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:1">
-      <x:c r="A81" s="1" t="s">
+      <x:c r="A81" s="2" t="s">
         <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:1">
-      <x:c r="A82" s="1" t="s">
+      <x:c r="A82" s="2" t="s">
         <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:1">
-      <x:c r="A83" s="1" t="s">
+      <x:c r="A83" s="2" t="s">
         <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:1">
-      <x:c r="A84" s="1" t="s">
+      <x:c r="A84" s="2" t="s">
         <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:1">
-      <x:c r="A85" s="1" t="s">
+      <x:c r="A85" s="2" t="s">
         <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:1">
-      <x:c r="A86" s="1" t="s">
+      <x:c r="A86" s="2" t="s">
         <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="87" spans="1:1">
-      <x:c r="A87" s="1" t="s">
+      <x:c r="A87" s="2" t="s">
         <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="1:1">
-      <x:c r="A88" s="1" t="s">
+      <x:c r="A88" s="2" t="s">
         <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="89" spans="1:1">
-      <x:c r="A89" s="1" t="s">
+      <x:c r="A89" s="2" t="s">
         <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:1">
-      <x:c r="A90" s="1" t="s">
+      <x:c r="A90" s="2" t="s">
         <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="91" spans="1:1">
-      <x:c r="A91" s="1" t="s">
+      <x:c r="A91" s="2" t="s">
         <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="92" spans="1:1">
-      <x:c r="A92" s="1" t="s">
+      <x:c r="A92" s="2" t="s">
         <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="93" spans="1:1">
-      <x:c r="A93" s="1" t="s">
+      <x:c r="A93" s="2" t="s">
         <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="94" spans="1:1">
-      <x:c r="A94" s="1" t="s">
+      <x:c r="A94" s="2" t="s">
         <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="95" spans="1:1">
-      <x:c r="A95" s="1" t="s">
+      <x:c r="A95" s="2" t="s">
         <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="96" spans="1:1">
-      <x:c r="A96" s="1" t="s">
+      <x:c r="A96" s="2" t="s">
         <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="97" spans="1:1">
-      <x:c r="A97" s="1" t="s">
+      <x:c r="A97" s="2" t="s">
         <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="98" spans="1:1">
-      <x:c r="A98" s="1" t="s">
+      <x:c r="A98" s="2" t="s">
         <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="99" spans="1:1">
-      <x:c r="A99" s="1" t="s">
+      <x:c r="A99" s="2" t="s">
         <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="1:1">
-      <x:c r="A100" s="1" t="s">
+      <x:c r="A100" s="2" t="s">
         <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="101" spans="1:1">
-      <x:c r="A101" s="1" t="s">
+      <x:c r="A101" s="2" t="s">
         <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="102" spans="1:1">
-      <x:c r="A102" s="1" t="s">
+      <x:c r="A102" s="2" t="s">
         <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="103" spans="1:1">
-      <x:c r="A103" s="1" t="s">
+      <x:c r="A103" s="2" t="s">
         <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="104" spans="1:1">
-      <x:c r="A104" s="1" t="s">
+      <x:c r="A104" s="2" t="s">
         <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="105" spans="1:1">
-      <x:c r="A105" s="1" t="s">
+      <x:c r="A105" s="2" t="s">
         <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="106" spans="1:1">
-      <x:c r="A106" s="1" t="s">
+      <x:c r="A106" s="2" t="s">
         <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="107" spans="1:1">
-      <x:c r="A107" s="1" t="s">
+      <x:c r="A107" s="2" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="108" spans="1:1">
-      <x:c r="A108" s="1" t="s">
+      <x:c r="A108" s="2" t="s">
         <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="109" spans="1:1">
-      <x:c r="A109" s="1" t="s">
+      <x:c r="A109" s="2" t="s">
         <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="110" spans="1:1">
-      <x:c r="A110" s="1" t="s">
+      <x:c r="A110" s="2" t="s">
         <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="111" spans="1:1">
-      <x:c r="A111" s="1" t="s">
+      <x:c r="A111" s="2" t="s">
         <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="112" spans="1:1">
-      <x:c r="A112" s="1" t="s">
+      <x:c r="A112" s="2" t="s">
         <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="113" spans="1:1">
-      <x:c r="A113" s="1" t="s">
+      <x:c r="A113" s="2" t="s">
         <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="114" spans="1:1">
-      <x:c r="A114" s="1" t="s">
+      <x:c r="A114" s="2" t="s">
         <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="115" spans="1:1">
-      <x:c r="A115" s="1" t="s">
+      <x:c r="A115" s="2" t="s">
         <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="116" spans="1:1">
-      <x:c r="A116" s="1" t="s">
+      <x:c r="A116" s="2" t="s">
         <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="117" spans="1:1">
-      <x:c r="A117" s="1" t="s">
+      <x:c r="A117" s="2" t="s">
         <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="118" spans="1:1">
-      <x:c r="A118" s="1" t="s">
+      <x:c r="A118" s="2" t="s">
         <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="119" spans="1:1">
-      <x:c r="A119" s="1" t="s">
+      <x:c r="A119" s="2" t="s">
         <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="120" spans="1:1">
-      <x:c r="A120" s="1" t="s">
+      <x:c r="A120" s="2" t="s">
         <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="121" spans="1:1">
-      <x:c r="A121" s="1" t="s">
+      <x:c r="A121" s="2" t="s">
         <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="122" spans="1:1">
-      <x:c r="A122" s="1" t="s">
+      <x:c r="A122" s="2" t="s">
         <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="123" spans="1:1">
-      <x:c r="A123" s="1" t="s">
+      <x:c r="A123" s="2" t="s">
         <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="124" spans="1:1">
-      <x:c r="A124" s="1" t="s">
+      <x:c r="A124" s="2" t="s">
         <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="125" spans="1:1">
-      <x:c r="A125" s="1" t="s">
+      <x:c r="A125" s="2" t="s">
         <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="126" spans="1:1">
-      <x:c r="A126" s="1" t="s">
+      <x:c r="A126" s="2" t="s">
         <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="127" spans="1:1">
-      <x:c r="A127" s="1" t="s">
+      <x:c r="A127" s="2" t="s">
         <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="128" spans="1:1">
-      <x:c r="A128" s="1" t="s">
+      <x:c r="A128" s="2" t="s">
         <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="129" spans="1:1">
-      <x:c r="A129" s="1" t="s">
+      <x:c r="A129" s="2" t="s">
         <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="130" spans="1:1">
-      <x:c r="A130" s="1" t="s">
+      <x:c r="A130" s="2" t="s">
         <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="131" spans="1:1">
-      <x:c r="A131" s="1" t="s">
+      <x:c r="A131" s="2" t="s">
         <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="132" spans="1:1">
-      <x:c r="A132" s="1" t="s">
+      <x:c r="A132" s="2" t="s">
         <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="133" spans="1:1">
-      <x:c r="A133" s="1" t="s">
+      <x:c r="A133" s="2" t="s">
         <x:v>126</x:v>
       </x:c>
     </x:row>
     <x:row r="134" spans="1:1">
-      <x:c r="A134" s="1" t="s">
+      <x:c r="A134" s="2" t="s">
         <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="135" spans="1:1">
-      <x:c r="A135" s="1" t="s">
+      <x:c r="A135" s="2" t="s">
         <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="136" spans="1:1">
-      <x:c r="A136" s="1" t="s">
+      <x:c r="A136" s="2" t="s">
         <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="137" spans="1:1">
-      <x:c r="A137" s="1" t="s">
+      <x:c r="A137" s="2" t="s">
         <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="138" spans="1:1">
-      <x:c r="A138" s="1" t="s">
+      <x:c r="A138" s="2" t="s">
         <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="139" spans="1:1">
-      <x:c r="A139" s="1" t="s">
+      <x:c r="A139" s="2" t="s">
         <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="140" spans="1:1">
-      <x:c r="A140" s="1" t="s">
+      <x:c r="A140" s="2" t="s">
         <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="141" spans="1:1">
-      <x:c r="A141" s="1" t="s">
+      <x:c r="A141" s="2" t="s">
         <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="142" spans="1:1">
-      <x:c r="A142" s="1" t="s">
+      <x:c r="A142" s="2" t="s">
         <x:v>135</x:v>
       </x:c>
     </x:row>
     <x:row r="143" spans="1:1">
-      <x:c r="A143" s="1" t="s">
+      <x:c r="A143" s="2" t="s">
         <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="144" spans="1:1">
-      <x:c r="A144" s="1" t="s">
+      <x:c r="A144" s="2" t="s">
         <x:v>137</x:v>
       </x:c>
     </x:row>
     <x:row r="145" spans="1:1">
-      <x:c r="A145" s="1" t="s">
+      <x:c r="A145" s="2" t="s">
         <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="146" spans="1:1">
-      <x:c r="A146" s="1" t="s">
+      <x:c r="A146" s="2" t="s">
         <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="147" spans="1:1">
-      <x:c r="A147" s="1" t="s">
+      <x:c r="A147" s="2" t="s">
         <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="148" spans="1:1">
-      <x:c r="A148" s="1" t="s">
+      <x:c r="A148" s="2" t="s">
         <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="149" spans="1:1">
-      <x:c r="A149" s="1" t="s">
+      <x:c r="A149" s="2" t="s">
         <x:v>142</x:v>
       </x:c>
     </x:row>
     <x:row r="150" spans="1:1">
-      <x:c r="A150" s="1" t="s">
+      <x:c r="A150" s="2" t="s">
         <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="151" spans="1:1">
-      <x:c r="A151" s="1" t="s">
+      <x:c r="A151" s="2" t="s">
         <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="152" spans="1:1">
-      <x:c r="A152" s="1" t="s">
+      <x:c r="A152" s="2" t="s">
         <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="153" spans="1:1">
-      <x:c r="A153" s="1" t="s">
+      <x:c r="A153" s="2" t="s">
         <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="154" spans="1:1">
-      <x:c r="A154" s="1" t="s">
+      <x:c r="A154" s="2" t="s">
         <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="155" spans="1:1">
-      <x:c r="A155" s="1" t="s">
+      <x:c r="A155" s="2" t="s">
         <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="156" spans="1:1">
-      <x:c r="A156" s="1" t="s">
+      <x:c r="A156" s="2" t="s">
         <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="157" spans="1:1">
-      <x:c r="A157" s="1" t="s">
+      <x:c r="A157" s="2" t="s">
         <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="158" spans="1:1">
-      <x:c r="A158" s="1" t="s">
+      <x:c r="A158" s="2" t="s">
         <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="159" spans="1:1">
-      <x:c r="A159" s="1" t="s">
+      <x:c r="A159" s="2" t="s">
         <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="160" spans="1:1">
-      <x:c r="A160" s="1" t="s">
+      <x:c r="A160" s="2" t="s">
         <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="161" spans="1:1">
-      <x:c r="A161" s="1" t="s">
+      <x:c r="A161" s="2" t="s">
         <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="162" spans="1:1">
-      <x:c r="A162" s="1" t="s">
+      <x:c r="A162" s="2" t="s">
         <x:v>155</x:v>
       </x:c>
     </x:row>
     <x:row r="163" spans="1:1">
-      <x:c r="A163" s="1" t="s">
+      <x:c r="A163" s="2" t="s">
         <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="164" spans="1:1">
-      <x:c r="A164" s="1" t="s">
+      <x:c r="A164" s="2" t="s">
         <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="165" spans="1:1">
-      <x:c r="A165" s="1" t="s">
+      <x:c r="A165" s="2" t="s">
         <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="166" spans="1:1">
-      <x:c r="A166" s="1" t="s">
+      <x:c r="A166" s="2" t="s">
         <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="167" spans="1:1">
-      <x:c r="A167" s="1" t="s">
+      <x:c r="A167" s="2" t="s">
         <x:v>160</x:v>
       </x:c>
     </x:row>
     <x:row r="168" spans="1:1">
-      <x:c r="A168" s="1" t="s">
+      <x:c r="A168" s="2" t="s">
         <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="169" spans="1:1">
-      <x:c r="A169" s="1" t="s">
+      <x:c r="A169" s="2" t="s">
         <x:v>162</x:v>
       </x:c>
     </x:row>
     <x:row r="170" spans="1:1">
-      <x:c r="A170" s="1" t="s">
+      <x:c r="A170" s="2" t="s">
         <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="171" spans="1:1">
-      <x:c r="A171" s="1" t="s">
+      <x:c r="A171" s="2" t="s">
         <x:v>164</x:v>
       </x:c>
     </x:row>
     <x:row r="172" spans="1:1">
-      <x:c r="A172" s="1" t="s">
+      <x:c r="A172" s="2" t="s">
         <x:v>165</x:v>
       </x:c>
     </x:row>
     <x:row r="173" spans="1:1">
-      <x:c r="A173" s="1" t="s">
+      <x:c r="A173" s="2" t="s">
         <x:v>166</x:v>
       </x:c>
     </x:row>
     <x:row r="174" spans="1:1">
-      <x:c r="A174" s="1" t="s">
+      <x:c r="A174" s="2" t="s">
         <x:v>167</x:v>
       </x:c>
     </x:row>
     <x:row r="175" spans="1:1">
-      <x:c r="A175" s="1" t="s">
+      <x:c r="A175" s="2" t="s">
         <x:v>168</x:v>
       </x:c>
     </x:row>
     <x:row r="176" spans="1:1">
-      <x:c r="A176" s="1" t="s">
+      <x:c r="A176" s="2" t="s">
         <x:v>169</x:v>
       </x:c>
     </x:row>
     <x:row r="177" spans="1:1">
-      <x:c r="A177" s="1" t="s">
+      <x:c r="A177" s="2" t="s">
         <x:v>170</x:v>
       </x:c>
     </x:row>
     <x:row r="178" spans="1:1">
-      <x:c r="A178" s="1" t="s">
+      <x:c r="A178" s="2" t="s">
         <x:v>171</x:v>
       </x:c>
     </x:row>
     <x:row r="179" spans="1:1">
-      <x:c r="A179" s="1" t="s">
+      <x:c r="A179" s="2" t="s">
         <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="180" spans="1:1">
-      <x:c r="A180" s="1" t="s">
+      <x:c r="A180" s="2" t="s">
         <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="181" spans="1:1">
-      <x:c r="A181" s="1" t="s">
+      <x:c r="A181" s="2" t="s">
         <x:v>174</x:v>
       </x:c>
     </x:row>
     <x:row r="182" spans="1:1">
-      <x:c r="A182" s="1" t="s">
+      <x:c r="A182" s="2" t="s">
         <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="183" spans="1:1">
-      <x:c r="A183" s="1" t="s">
+      <x:c r="A183" s="2" t="s">
         <x:v>169</x:v>
       </x:c>
     </x:row>
     <x:row r="184" spans="1:1">
-      <x:c r="A184" s="1" t="s">
+      <x:c r="A184" s="2" t="s">
         <x:v>176</x:v>
       </x:c>
     </x:row>
     <x:row r="185" spans="1:1">
-      <x:c r="A185" s="1" t="s">
+      <x:c r="A185" s="2" t="s">
         <x:v>177</x:v>
       </x:c>
     </x:row>
     <x:row r="186" spans="1:1">
-      <x:c r="A186" s="1" t="s">
+      <x:c r="A186" s="2" t="s">
         <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="187" spans="1:1">
-      <x:c r="A187" s="1" t="s">
+      <x:c r="A187" s="2" t="s">
         <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="188" spans="1:1">
-      <x:c r="A188" s="1" t="s">
+      <x:c r="A188" s="2" t="s">
         <x:v>180</x:v>
       </x:c>
     </x:row>
     <x:row r="189" spans="1:1">
-      <x:c r="A189" s="1" t="s">
+      <x:c r="A189" s="2" t="s">
         <x:v>181</x:v>
       </x:c>
     </x:row>
     <x:row r="190" spans="1:1">
-      <x:c r="A190" s="1" t="s">
+      <x:c r="A190" s="2" t="s">
         <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="191" spans="1:1">
-      <x:c r="A191" s="1" t="s">
+      <x:c r="A191" s="2" t="s">
         <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="192" spans="1:1">
-      <x:c r="A192" s="1" t="s">
+      <x:c r="A192" s="2" t="s">
         <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="193" spans="1:1">
-      <x:c r="A193" s="1" t="s">
+      <x:c r="A193" s="2" t="s">
         <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="194" spans="1:1">
-      <x:c r="A194" s="1" t="s">
+      <x:c r="A194" s="2" t="s">
         <x:v>186</x:v>
       </x:c>
     </x:row>
     <x:row r="195" spans="1:1">
-      <x:c r="A195" s="1" t="s">
+      <x:c r="A195" s="2" t="s">
         <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="196" spans="1:1">
-      <x:c r="A196" s="1" t="s">
+      <x:c r="A196" s="2" t="s">
         <x:v>188</x:v>
       </x:c>
     </x:row>
     <x:row r="197" spans="1:1">
-      <x:c r="A197" s="1" t="s">
+      <x:c r="A197" s="2" t="s">
         <x:v>189</x:v>
       </x:c>
     </x:row>
     <x:row r="198" spans="1:1">
-      <x:c r="A198" s="1" t="s">
+      <x:c r="A198" s="2" t="s">
         <x:v>190</x:v>
       </x:c>
     </x:row>
     <x:row r="199" spans="1:1">
-      <x:c r="A199" s="1" t="s">
+      <x:c r="A199" s="2" t="s">
         <x:v>191</x:v>
       </x:c>
     </x:row>
     <x:row r="200" spans="1:1">
-      <x:c r="A200" s="1" t="s">
+      <x:c r="A200" s="2" t="s">
         <x:v>192</x:v>
       </x:c>
     </x:row>
     <x:row r="201" spans="1:1">
-      <x:c r="A201" s="1" t="s">
+      <x:c r="A201" s="2" t="s">
         <x:v>193</x:v>
       </x:c>
     </x:row>
     <x:row r="202" spans="1:1">
-      <x:c r="A202" s="1" t="s">
+      <x:c r="A202" s="2" t="s">
         <x:v>194</x:v>
       </x:c>
     </x:row>
     <x:row r="203" spans="1:1">
-      <x:c r="A203" s="1" t="s">
+      <x:c r="A203" s="2" t="s">
         <x:v>195</x:v>
       </x:c>
     </x:row>
     <x:row r="204" spans="1:1">
-      <x:c r="A204" s="1" t="s">
+      <x:c r="A204" s="2" t="s">
         <x:v>196</x:v>
       </x:c>
     </x:row>
     <x:row r="205" spans="1:1">
-      <x:c r="A205" s="1" t="s">
+      <x:c r="A205" s="2" t="s">
         <x:v>197</x:v>
       </x:c>
     </x:row>
     <x:row r="206" spans="1:1">
-      <x:c r="A206" s="1" t="s">
+      <x:c r="A206" s="2" t="s">
         <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="207" spans="1:1">
-      <x:c r="A207" s="1" t="s">
+      <x:c r="A207" s="2" t="s">
         <x:v>199</x:v>
       </x:c>
     </x:row>
     <x:row r="208" spans="1:1">
-      <x:c r="A208" s="1" t="s">
+      <x:c r="A208" s="2" t="s">
         <x:v>200</x:v>
       </x:c>
     </x:row>
     <x:row r="209" spans="1:1">
-      <x:c r="A209" s="1" t="s">
+      <x:c r="A209" s="2" t="s">
         <x:v>201</x:v>
       </x:c>
     </x:row>
     <x:row r="210" spans="1:1">
-      <x:c r="A210" s="1" t="s">
+      <x:c r="A210" s="2" t="s">
         <x:v>202</x:v>
       </x:c>
     </x:row>
     <x:row r="211" spans="1:1">
-      <x:c r="A211" s="1" t="s">
+      <x:c r="A211" s="2" t="s">
         <x:v>203</x:v>
       </x:c>
     </x:row>
     <x:row r="212" spans="1:1">
-      <x:c r="A212" s="1" t="s">
+      <x:c r="A212" s="2" t="s">
         <x:v>204</x:v>
       </x:c>
     </x:row>
     <x:row r="213" spans="1:1">
-      <x:c r="A213" s="1" t="s">
+      <x:c r="A213" s="2" t="s">
         <x:v>205</x:v>
       </x:c>
     </x:row>
     <x:row r="214" spans="1:1">
-      <x:c r="A214" s="1" t="s">
+      <x:c r="A214" s="2" t="s">
         <x:v>206</x:v>
       </x:c>
     </x:row>
     <x:row r="215" spans="1:1">
-      <x:c r="A215" s="1" t="s">
+      <x:c r="A215" s="2" t="s">
         <x:v>207</x:v>
       </x:c>
     </x:row>
     <x:row r="216" spans="1:1">
-      <x:c r="A216" s="1" t="s">
+      <x:c r="A216" s="2" t="s">
         <x:v>208</x:v>
       </x:c>
     </x:row>
     <x:row r="217" spans="1:1">
-      <x:c r="A217" s="1" t="s">
+      <x:c r="A217" s="2" t="s">
         <x:v>209</x:v>
       </x:c>
     </x:row>
     <x:row r="218" spans="1:1">
-      <x:c r="A218" s="1" t="s">
+      <x:c r="A218" s="2" t="s">
         <x:v>210</x:v>
       </x:c>
     </x:row>
     <x:row r="219" spans="1:1">
-      <x:c r="A219" s="1" t="s">
+      <x:c r="A219" s="2" t="s">
         <x:v>211</x:v>
       </x:c>
     </x:row>
     <x:row r="220" spans="1:1">
-      <x:c r="A220" s="1" t="s">
+      <x:c r="A220" s="2" t="s">
         <x:v>212</x:v>
       </x:c>
     </x:row>
     <x:row r="221" spans="1:1">
-      <x:c r="A221" s="1" t="s">
+      <x:c r="A221" s="2" t="s">
         <x:v>213</x:v>
       </x:c>
     </x:row>
     <x:row r="222" spans="1:1">
-      <x:c r="A222" s="1" t="s">
+      <x:c r="A222" s="2" t="s">
         <x:v>214</x:v>
       </x:c>
     </x:row>
     <x:row r="223" spans="1:1">
-      <x:c r="A223" s="1" t="s">
+      <x:c r="A223" s="2" t="s">
         <x:v>215</x:v>
       </x:c>
     </x:row>
     <x:row r="224" spans="1:1">
-      <x:c r="A224" s="1" t="s">
+      <x:c r="A224" s="2" t="s">
         <x:v>216</x:v>
       </x:c>
     </x:row>
     <x:row r="225" spans="1:1">
-      <x:c r="A225" s="1" t="s">
+      <x:c r="A225" s="2" t="s">
         <x:v>217</x:v>
       </x:c>
     </x:row>
     <x:row r="226" spans="1:1">
-      <x:c r="A226" s="1" t="s">
+      <x:c r="A226" s="2" t="s">
         <x:v>218</x:v>
       </x:c>
     </x:row>
     <x:row r="227" spans="1:1">
-      <x:c r="A227" s="1" t="s">
+      <x:c r="A227" s="2" t="s">
         <x:v>219</x:v>
       </x:c>
     </x:row>
     <x:row r="228" spans="1:1">
-      <x:c r="A228" s="1" t="s">
+      <x:c r="A228" s="2" t="s">
         <x:v>220</x:v>
       </x:c>
     </x:row>
     <x:row r="229" spans="1:1">
-      <x:c r="A229" s="1" t="s">
+      <x:c r="A229" s="2" t="s">
         <x:v>221</x:v>
       </x:c>
     </x:row>
     <x:row r="230" spans="1:1">
-      <x:c r="A230" s="1" t="s">
+      <x:c r="A230" s="2" t="s">
         <x:v>222</x:v>
       </x:c>
     </x:row>
     <x:row r="231" spans="1:1">
-      <x:c r="A231" s="1" t="s">
+      <x:c r="A231" s="2" t="s">
         <x:v>223</x:v>
       </x:c>
     </x:row>
     <x:row r="232" spans="1:1">
-      <x:c r="A232" s="1" t="s">
+      <x:c r="A232" s="2" t="s">
         <x:v>224</x:v>
       </x:c>
     </x:row>
     <x:row r="233" spans="1:1">
-      <x:c r="A233" s="1" t="s">
+      <x:c r="A233" s="2" t="s">
         <x:v>225</x:v>
       </x:c>
     </x:row>
     <x:row r="234" spans="1:1">
-      <x:c r="A234" s="1" t="s">
+      <x:c r="A234" s="2" t="s">
         <x:v>226</x:v>
       </x:c>
     </x:row>
     <x:row r="235" spans="1:1">
-      <x:c r="A235" s="1" t="s">
+      <x:c r="A235" s="2" t="s">
         <x:v>227</x:v>
       </x:c>
     </x:row>
     <x:row r="236" spans="1:1">
-      <x:c r="A236" s="1" t="s">
+      <x:c r="A236" s="2" t="s">
         <x:v>228</x:v>
       </x:c>
     </x:row>
     <x:row r="237" spans="1:1">
-      <x:c r="A237" s="1" t="s">
+      <x:c r="A237" s="2" t="s">
         <x:v>229</x:v>
       </x:c>
     </x:row>
     <x:row r="238" spans="1:1">
-      <x:c r="A238" s="1" t="s">
+      <x:c r="A238" s="2" t="s">
         <x:v>230</x:v>
       </x:c>
     </x:row>
     <x:row r="239" spans="1:1">
-      <x:c r="A239" s="1" t="s">
+      <x:c r="A239" s="2" t="s">
         <x:v>231</x:v>
       </x:c>
     </x:row>
     <x:row r="240" spans="1:1">
-      <x:c r="A240" s="1" t="s">
+      <x:c r="A240" s="2" t="s">
         <x:v>232</x:v>
       </x:c>
     </x:row>
     <x:row r="241" spans="1:1">
-      <x:c r="A241" s="1" t="s">
+      <x:c r="A241" s="2" t="s">
         <x:v>233</x:v>
       </x:c>
     </x:row>
     <x:row r="242" spans="1:1">
-      <x:c r="A242" s="1" t="s">
+      <x:c r="A242" s="2" t="s">
         <x:v>234</x:v>
       </x:c>
     </x:row>
     <x:row r="243" spans="1:1">
-      <x:c r="A243" s="1" t="s">
+      <x:c r="A243" s="2" t="s">
         <x:v>235</x:v>
       </x:c>
     </x:row>
     <x:row r="244" spans="1:1">
-      <x:c r="A244" s="1" t="s">
+      <x:c r="A244" s="2" t="s">
         <x:v>236</x:v>
       </x:c>
     </x:row>
     <x:row r="245" spans="1:1">
-      <x:c r="A245" s="1" t="s">
+      <x:c r="A245" s="2" t="s">
         <x:v>237</x:v>
       </x:c>
     </x:row>
     <x:row r="246" spans="1:1">
-      <x:c r="A246" s="1" t="s">
+      <x:c r="A246" s="2" t="s">
         <x:v>238</x:v>
       </x:c>
     </x:row>
     <x:row r="247" spans="1:1">
-      <x:c r="A247" s="1" t="s">
+      <x:c r="A247" s="2" t="s">
         <x:v>239</x:v>
       </x:c>
     </x:row>
     <x:row r="248" spans="1:1">
-      <x:c r="A248" s="1" t="s">
+      <x:c r="A248" s="2" t="s">
         <x:v>240</x:v>
       </x:c>
     </x:row>
     <x:row r="249" spans="1:1">
-      <x:c r="A249" s="1" t="s">
+      <x:c r="A249" s="2" t="s">
         <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="250" spans="1:1">
-      <x:c r="A250" s="1" t="s">
+      <x:c r="A250" s="2" t="s">
         <x:v>242</x:v>
       </x:c>
     </x:row>
     <x:row r="251" spans="1:1">
-      <x:c r="A251" s="1" t="s">
+      <x:c r="A251" s="2" t="s">
         <x:v>243</x:v>
       </x:c>
     </x:row>
     <x:row r="252" spans="1:1">
-      <x:c r="A252" s="1" t="s">
+      <x:c r="A252" s="2" t="s">
         <x:v>244</x:v>
       </x:c>
     </x:row>
     <x:row r="253" spans="1:1">
-      <x:c r="A253" s="1" t="s">
+      <x:c r="A253" s="2" t="s">
         <x:v>245</x:v>
       </x:c>
     </x:row>
     <x:row r="254" spans="1:1">
-      <x:c r="A254" s="1" t="s">
+      <x:c r="A254" s="2" t="s">
         <x:v>246</x:v>
       </x:c>
     </x:row>
     <x:row r="255" spans="1:1">
-      <x:c r="A255" s="1" t="s">
+      <x:c r="A255" s="2" t="s">
         <x:v>247</x:v>
       </x:c>
     </x:row>
     <x:row r="256" spans="1:1">
-      <x:c r="A256" s="1" t="s">
+      <x:c r="A256" s="2" t="s">
         <x:v>248</x:v>
       </x:c>
     </x:row>
     <x:row r="257" spans="1:1">
-      <x:c r="A257" s="1" t="s">
+      <x:c r="A257" s="2" t="s">
         <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="258" spans="1:1">
-      <x:c r="A258" s="1" t="s">
+      <x:c r="A258" s="2" t="s">
         <x:v>250</x:v>
       </x:c>
     </x:row>
     <x:row r="259" spans="1:1">
-      <x:c r="A259" s="1" t="s">
+      <x:c r="A259" s="2" t="s">
         <x:v>251</x:v>
       </x:c>
     </x:row>
     <x:row r="260" spans="1:1">
-      <x:c r="A260" s="1" t="s">
+      <x:c r="A260" s="2" t="s">
         <x:v>252</x:v>
       </x:c>
     </x:row>
     <x:row r="261" spans="1:1">
-      <x:c r="A261" s="1" t="s">
+      <x:c r="A261" s="2" t="s">
         <x:v>253</x:v>
       </x:c>
     </x:row>
     <x:row r="262" spans="1:1">
-      <x:c r="A262" s="1" t="s">
+      <x:c r="A262" s="2" t="s">
         <x:v>254</x:v>
       </x:c>
     </x:row>
     <x:row r="263" spans="1:1">
-      <x:c r="A263" s="1" t="s">
+      <x:c r="A263" s="2" t="s">
         <x:v>255</x:v>
       </x:c>
     </x:row>
     <x:row r="264" spans="1:1">
-      <x:c r="A264" s="1" t="s">
+      <x:c r="A264" s="2" t="s">
         <x:v>256</x:v>
       </x:c>
     </x:row>
     <x:row r="265" spans="1:1">
-      <x:c r="A265" s="1" t="s">
+      <x:c r="A265" s="2" t="s">
         <x:v>257</x:v>
       </x:c>
     </x:row>
     <x:row r="266" spans="1:1">
-      <x:c r="A266" s="1" t="s">
+      <x:c r="A266" s="2" t="s">
         <x:v>258</x:v>
       </x:c>
     </x:row>
     <x:row r="267" spans="1:1">
-      <x:c r="A267" s="1" t="s">
+      <x:c r="A267" s="2" t="s">
         <x:v>259</x:v>
       </x:c>
     </x:row>
     <x:row r="268" spans="1:1">
-      <x:c r="A268" s="1" t="s">
+      <x:c r="A268" s="2" t="s">
         <x:v>260</x:v>
       </x:c>
     </x:row>
     <x:row r="269" spans="1:1">
-      <x:c r="A269" s="1" t="s">
+      <x:c r="A269" s="2" t="s">
         <x:v>261</x:v>
       </x:c>
     </x:row>
     <x:row r="270" spans="1:1">
-      <x:c r="A270" s="1" t="s">
+      <x:c r="A270" s="2" t="s">
         <x:v>262</x:v>
       </x:c>
     </x:row>
     <x:row r="271" spans="1:1">
-      <x:c r="A271" s="1" t="s">
+      <x:c r="A271" s="2" t="s">
         <x:v>263</x:v>
       </x:c>
     </x:row>
     <x:row r="272" spans="1:1">
-      <x:c r="A272" s="1" t="s">
+      <x:c r="A272" s="2" t="s">
         <x:v>264</x:v>
       </x:c>
     </x:row>
     <x:row r="273" spans="1:1">
-      <x:c r="A273" s="1" t="s">
+      <x:c r="A273" s="2" t="s">
         <x:v>265</x:v>
       </x:c>
     </x:row>
     <x:row r="274" spans="1:1">
-      <x:c r="A274" s="1" t="s">
+      <x:c r="A274" s="2" t="s">
         <x:v>266</x:v>
       </x:c>
     </x:row>
     <x:row r="275" spans="1:1">
-      <x:c r="A275" s="1" t="s">
+      <x:c r="A275" s="2" t="s">
         <x:v>267</x:v>
       </x:c>
     </x:row>
     <x:row r="276" spans="1:1">
-      <x:c r="A276" s="1" t="s">
+      <x:c r="A276" s="2" t="s">
         <x:v>268</x:v>
       </x:c>
     </x:row>
     <x:row r="277" spans="1:1">
-      <x:c r="A277" s="1" t="s">
+      <x:c r="A277" s="2" t="s">
         <x:v>269</x:v>
       </x:c>
     </x:row>
     <x:row r="278" spans="1:1">
-      <x:c r="A278" s="1" t="s">
+      <x:c r="A278" s="2" t="s">
         <x:v>270</x:v>
       </x:c>
     </x:row>
     <x:row r="279" spans="1:1">
-      <x:c r="A279" s="1" t="s">
+      <x:c r="A279" s="2" t="s">
         <x:v>271</x:v>
       </x:c>
     </x:row>
     <x:row r="280" spans="1:1">
-      <x:c r="A280" s="1" t="s">
+      <x:c r="A280" s="2" t="s">
         <x:v>272</x:v>
       </x:c>
     </x:row>
     <x:row r="281" spans="1:1">
-      <x:c r="A281" s="1" t="s">
+      <x:c r="A281" s="2" t="s">
         <x:v>273</x:v>
       </x:c>
     </x:row>
     <x:row r="282" spans="1:1">
-      <x:c r="A282" s="1" t="s">
+      <x:c r="A282" s="2" t="s">
         <x:v>274</x:v>
       </x:c>
     </x:row>
     <x:row r="283" spans="1:1">
-      <x:c r="A283" s="1" t="s">
+      <x:c r="A283" s="2" t="s">
         <x:v>275</x:v>
       </x:c>
     </x:row>
     <x:row r="284" spans="1:1">
-      <x:c r="A284" s="1" t="s">
+      <x:c r="A284" s="2" t="s">
         <x:v>276</x:v>
       </x:c>
     </x:row>
     <x:row r="285" spans="1:1">
-      <x:c r="A285" s="1" t="s">
+      <x:c r="A285" s="2" t="s">
         <x:v>277</x:v>
       </x:c>
     </x:row>
     <x:row r="286" spans="1:1">
-      <x:c r="A286" s="1" t="s">
+      <x:c r="A286" s="2" t="s">
         <x:v>278</x:v>
       </x:c>
     </x:row>
     <x:row r="287" spans="1:1">
-      <x:c r="A287" s="1" t="s">
+      <x:c r="A287" s="2" t="s">
         <x:v>279</x:v>
       </x:c>
     </x:row>
     <x:row r="288" spans="1:1">
-      <x:c r="A288" s="1" t="s">
+      <x:c r="A288" s="2" t="s">
         <x:v>280</x:v>
       </x:c>
     </x:row>
     <x:row r="289" spans="1:1">
-      <x:c r="A289" s="1" t="s">
+      <x:c r="A289" s="2" t="s">
         <x:v>281</x:v>
       </x:c>
     </x:row>
     <x:row r="290" spans="1:1">
-      <x:c r="A290" s="1" t="s">
+      <x:c r="A290" s="2" t="s">
         <x:v>282</x:v>
       </x:c>
     </x:row>
     <x:row r="291" spans="1:1">
-      <x:c r="A291" s="1" t="s">
+      <x:c r="A291" s="2" t="s">
         <x:v>283</x:v>
       </x:c>
     </x:row>
     <x:row r="292" spans="1:1">
-      <x:c r="A292" s="1" t="s">
+      <x:c r="A292" s="2" t="s">
         <x:v>284</x:v>
       </x:c>
     </x:row>
     <x:row r="293" spans="1:1">
-      <x:c r="A293" s="1" t="s">
+      <x:c r="A293" s="2" t="s">
         <x:v>285</x:v>
       </x:c>
     </x:row>
     <x:row r="294" spans="1:1">
-      <x:c r="A294" s="1" t="s">
+      <x:c r="A294" s="2" t="s">
         <x:v>286</x:v>
       </x:c>
     </x:row>
     <x:row r="295" spans="1:1">
-      <x:c r="A295" s="1" t="s">
+      <x:c r="A295" s="2" t="s">
         <x:v>287</x:v>
       </x:c>
     </x:row>
     <x:row r="296" spans="1:1">
-      <x:c r="A296" s="1" t="s">
+      <x:c r="A296" s="2" t="s">
         <x:v>288</x:v>
       </x:c>
     </x:row>
     <x:row r="297" spans="1:1">
-      <x:c r="A297" s="1" t="s">
+      <x:c r="A297" s="2" t="s">
         <x:v>289</x:v>
       </x:c>
     </x:row>
     <x:row r="298" spans="1:1">
-      <x:c r="A298" s="1" t="s">
+      <x:c r="A298" s="2" t="s">
         <x:v>290</x:v>
       </x:c>
     </x:row>
     <x:row r="299" spans="1:1">
-      <x:c r="A299" s="1" t="s">
+      <x:c r="A299" s="2" t="s">
         <x:v>291</x:v>
       </x:c>
     </x:row>
     <x:row r="300" spans="1:1">
-      <x:c r="A300" s="1" t="s">
+      <x:c r="A300" s="2" t="s">
         <x:v>292</x:v>
       </x:c>
     </x:row>
     <x:row r="301" spans="1:1">
-      <x:c r="A301" s="1" t="s">
+      <x:c r="A301" s="2" t="s">
         <x:v>293</x:v>
       </x:c>
     </x:row>
     <x:row r="302" spans="1:1">
-      <x:c r="A302" s="1" t="s">
+      <x:c r="A302" s="2" t="s">
         <x:v>294</x:v>
       </x:c>
     </x:row>
     <x:row r="303" spans="1:1">
-      <x:c r="A303" s="1" t="s">
+      <x:c r="A303" s="2" t="s">
         <x:v>295</x:v>
       </x:c>
     </x:row>
     <x:row r="304" spans="1:1">
-      <x:c r="A304" s="1" t="s">
+      <x:c r="A304" s="2" t="s">
         <x:v>296</x:v>
       </x:c>
     </x:row>
     <x:row r="305" spans="1:1">
-      <x:c r="A305" s="1" t="s">
+      <x:c r="A305" s="2" t="s">
         <x:v>297</x:v>
       </x:c>
     </x:row>
     <x:row r="306" spans="1:1">
-      <x:c r="A306" s="1" t="s">
+      <x:c r="A306" s="2" t="s">
         <x:v>298</x:v>
       </x:c>
     </x:row>
     <x:row r="307" spans="1:1">
-      <x:c r="A307" s="1" t="s">
+      <x:c r="A307" s="2" t="s">
         <x:v>299</x:v>
       </x:c>
     </x:row>
     <x:row r="308" spans="1:1">
-      <x:c r="A308" s="1" t="s">
+      <x:c r="A308" s="2" t="s">
         <x:v>300</x:v>
       </x:c>
     </x:row>
     <x:row r="309" spans="1:1">
-      <x:c r="A309" s="1" t="s">
+      <x:c r="A309" s="2" t="s">
         <x:v>301</x:v>
       </x:c>
     </x:row>
     <x:row r="310" spans="1:1">
-      <x:c r="A310" s="1" t="s">
+      <x:c r="A310" s="2" t="s">
         <x:v>302</x:v>
       </x:c>
     </x:row>
     <x:row r="311" spans="1:1">
-      <x:c r="A311" s="1" t="s">
+      <x:c r="A311" s="2" t="s">
         <x:v>303</x:v>
       </x:c>
     </x:row>
     <x:row r="312" spans="1:1">
-      <x:c r="A312" s="1" t="s">
+      <x:c r="A312" s="2" t="s">
         <x:v>304</x:v>
       </x:c>
     </x:row>
     <x:row r="313" spans="1:1">
-      <x:c r="A313" s="1" t="s">
+      <x:c r="A313" s="2" t="s">
         <x:v>305</x:v>
       </x:c>
     </x:row>
     <x:row r="314" spans="1:1">
-      <x:c r="A314" s="1" t="s">
+      <x:c r="A314" s="2" t="s">
         <x:v>306</x:v>
       </x:c>
     </x:row>
     <x:row r="315" spans="1:1">
-      <x:c r="A315" s="1" t="s">
+      <x:c r="A315" s="2" t="s">
         <x:v>307</x:v>
       </x:c>
     </x:row>
     <x:row r="316" spans="1:1">
-      <x:c r="A316" s="1" t="s">
+      <x:c r="A316" s="2" t="s">
         <x:v>308</x:v>
       </x:c>
     </x:row>
     <x:row r="317" spans="1:1">
-      <x:c r="A317" s="1" t="s">
+      <x:c r="A317" s="2" t="s">
         <x:v>309</x:v>
       </x:c>
     </x:row>
     <x:row r="318" spans="1:1">
-      <x:c r="A318" s="1" t="s">
+      <x:c r="A318" s="2" t="s">
         <x:v>310</x:v>
       </x:c>
     </x:row>
     <x:row r="319" spans="1:1">
-      <x:c r="A319" s="1" t="s">
+      <x:c r="A319" s="2" t="s">
         <x:v>311</x:v>
       </x:c>
     </x:row>
     <x:row r="320" spans="1:1">
-      <x:c r="A320" s="1" t="s">
+      <x:c r="A320" s="2" t="s">
         <x:v>312</x:v>
       </x:c>
     </x:row>
     <x:row r="321" spans="1:1">
-      <x:c r="A321" s="1" t="s">
+      <x:c r="A321" s="2" t="s">
         <x:v>313</x:v>
       </x:c>
     </x:row>
     <x:row r="322" spans="1:1">
-      <x:c r="A322" s="1" t="s">
+      <x:c r="A322" s="2" t="s">
         <x:v>314</x:v>
       </x:c>
     </x:row>
     <x:row r="323" spans="1:1">
-      <x:c r="A323" s="1" t="s">
+      <x:c r="A323" s="2" t="s">
         <x:v>315</x:v>
       </x:c>
     </x:row>
     <x:row r="324" spans="1:1">
-      <x:c r="A324" s="1" t="s">
+      <x:c r="A324" s="2" t="s">
         <x:v>316</x:v>
       </x:c>
     </x:row>
     <x:row r="325" spans="1:1">
-      <x:c r="A325" s="1" t="s">
+      <x:c r="A325" s="2" t="s">
         <x:v>317</x:v>
       </x:c>
     </x:row>
     <x:row r="326" spans="1:1">
-      <x:c r="A326" s="1" t="s">
+      <x:c r="A326" s="2" t="s">
         <x:v>318</x:v>
       </x:c>
     </x:row>
     <x:row r="327" spans="1:1">
-      <x:c r="A327" s="1" t="s">
+      <x:c r="A327" s="2" t="s">
         <x:v>319</x:v>
       </x:c>
     </x:row>
     <x:row r="328" spans="1:1">
-      <x:c r="A328" s="1" t="s">
+      <x:c r="A328" s="2" t="s">
         <x:v>320</x:v>
       </x:c>
     </x:row>
     <x:row r="329" spans="1:1">
-      <x:c r="A329" s="1" t="s">
+      <x:c r="A329" s="2" t="s">
         <x:v>321</x:v>
       </x:c>
     </x:row>
     <x:row r="330" spans="1:1">
-      <x:c r="A330" s="1" t="s">
+      <x:c r="A330" s="2" t="s">
         <x:v>322</x:v>
       </x:c>
     </x:row>
     <x:row r="331" spans="1:1">
-      <x:c r="A331" s="1" t="s">
+      <x:c r="A331" s="2" t="s">
         <x:v>323</x:v>
       </x:c>
     </x:row>
     <x:row r="332" spans="1:1">
-      <x:c r="A332" s="1" t="s">
+      <x:c r="A332" s="2" t="s">
         <x:v>324</x:v>
       </x:c>
     </x:row>
     <x:row r="333" spans="1:1">
-      <x:c r="A333" s="1" t="s">
+      <x:c r="A333" s="2" t="s">
         <x:v>325</x:v>
       </x:c>
     </x:row>

</xml_diff>